<commit_message>
classe para listar na tela as fisioterapeutas cadastradas
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -4,31 +4,52 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="pacientes" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="pesquisadores" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="fisioterapeutas" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="administradores" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="f" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Cambria"/>
+      <charset val="1"/>
+      <family val="0"/>
       <b val="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,21 +73,45 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -139,41 +184,41 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="ffffff"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="1f497d"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="eeece1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4f81bd"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="c0504d"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="9bbb59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="8064a2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4bacc6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="f79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0000ff"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -181,290 +226,367 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="1" sqref="A4:B4 F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Senha</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Maria</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>maria</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>maria</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:B4 A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Senha</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Joana</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>joana</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>joana</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr filterMode="0">
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr fitToPage="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="A4:B4 B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1" s="3">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Login</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Senha</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15" customHeight="1" s="3">
+      <c r="A2" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" s="5" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>mario</t>
+        </is>
+      </c>
+      <c r="D2" s="5" t="inlineStr">
+        <is>
+          <t>mario</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -493,35 +615,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Nome</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
correções nos métodos listar
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -409,7 +409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,10 +460,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="A3" t="n">
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -478,6 +476,48 @@
       <c r="D3" t="inlineStr">
         <is>
           <t>carlos</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Ulises</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ulises</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>ulises</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>jose</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>jose</t>
         </is>
       </c>
     </row>
@@ -488,45 +528,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:B4 A1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="6" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="6" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>Login</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="6" t="inlineStr">
         <is>
           <t>Senha</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15" customHeight="1" s="3">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
@@ -544,10 +582,50 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>Abraoo</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>abraoo</t>
+        </is>
+      </c>
+      <c r="D3" s="5" t="inlineStr">
+        <is>
+          <t>abraoo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Jose</t>
+        </is>
+      </c>
+      <c r="C4" s="5" t="inlineStr">
+        <is>
+          <t>jose</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>jose</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Criação da classe agendapaciente para organizar as datas do tramento e suas respectivas entradas nas classes cadastro paciente e paciente
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -372,34 +372,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="1" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1" s="3">
-      <c r="A1" s="4" t="inlineStr">
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Nome</t>
         </is>
       </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>Data Nascimento</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Data Inicio</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mario</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>23/11/2000</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>15/11/2025</t>
+        </is>
+      </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -503,22 +533,22 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="6" t="inlineStr">
         <is>
           <t>Fisio</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="6" t="inlineStr">
         <is>
           <t>fisio</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="6" t="inlineStr">
         <is>
           <t>fisio</t>
         </is>

</xml_diff>